<commit_message>
reopening - facemask mandated (amended)
</commit_message>
<xml_diff>
--- a/covid-19_dist0720_0716CSD.xlsx
+++ b/covid-19_dist0720_0716CSD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SumiKim\Desktop\MIDS_Courses\W203_Statistics\Lab3\Lab-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F374EB0-233D-46DA-B85E-69F682E3BE70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D3AE95-3C23-422C-AD65-DDF70D4699D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Mtest2" sheetId="9" r:id="rId2"/>
     <sheet name="Mtest3" sheetId="10" r:id="rId3"/>
     <sheet name="Mtest4" sheetId="11" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId5"/>
+    <sheet name="Mtest5" sheetId="12" r:id="rId5"/>
     <sheet name="test1" sheetId="4" r:id="rId6"/>
     <sheet name="Infromation" sheetId="1" r:id="rId7"/>
     <sheet name="Covid-19" sheetId="2" r:id="rId8"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="176">
   <si>
     <t>Variables</t>
   </si>
@@ -583,34 +583,7 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>요약 출력</t>
-  </si>
-  <si>
-    <t>회귀분석 통계량</t>
-  </si>
-  <si>
-    <t>다중 상관계수</t>
-  </si>
-  <si>
-    <t>결정계수</t>
-  </si>
-  <si>
-    <t>조정된 결정계수</t>
-  </si>
-  <si>
     <t>표준 오차</t>
-  </si>
-  <si>
-    <t>분산 분석</t>
-  </si>
-  <si>
-    <t>회귀</t>
-  </si>
-  <si>
-    <t>계</t>
-  </si>
-  <si>
-    <t>Y 절편</t>
   </si>
   <si>
     <t>자유도</t>
@@ -1298,6 +1271,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1325,7 +1299,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7079,7 +7052,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$26:$B$76</c:f>
+              <c:f>Mtest5!$B$26:$B$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -7906,7 +7879,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$26:$B$76</c:f>
+              <c:f>Mtest5!$B$26:$B$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -18914,6 +18887,694 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>Reopen-MaskMandate</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:t> (X) vs. </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:t>Log(7D/Population)(Y)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.24933198208640944"/>
+          <c:y val="2.5598394874101392E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.38261613220359869"/>
+                  <c:y val="4.260908976254249E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ko-KR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>test1!$AJ$2:$AJ$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-62</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-48</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-59</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-59</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-66</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-49</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-69</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-73</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-62</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-52</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>test1!$AC$2:$AC$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>-2.697716432967173</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.4144071728882381</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.4078718127782115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.8255196492339185</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.8670716688499676</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.445268369677275</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3.8445713952526472</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.9460891468312589</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.421736871479641</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.502394762167123</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.7095839628407377</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.0157179192920447</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2.8613438214993216</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-3.3098129076803535</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-3.2898742112899257</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2.975280471767852</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-3.0873581448645275</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-3.5677259366643019</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-2.6489767583489803</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-3.76109924101273</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.2861044459359259</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.6540091396816257</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3.4863385977541657</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3.2690471802236352</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-2.7455971553356227</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.2854653055889269</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-3.4274587188333623</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-3.2231867520728406</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-2.6988829936285605</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-3.7782979121012459</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-3.5468567299986686</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-3.1072240634291677</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-3.5834034775676691</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-2.9213189896141936</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-3.3269745642963731</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-3.1815287214131085</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-3.063208477066846</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-3.2926866709396818</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-3.4254849851668485</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-3.5056904536559634</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-2.595357433834272</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-3.3051028461311707</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-2.779089491050422</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-2.7430103125945386</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-2.8452773669640958</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-4.0892115421739792</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-3.2902378436354032</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-3.2244842506741875</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-3.5139522133069376</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-3.109977423156308</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-3.3779148159651173</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5713-4EBA-B716-806941DC5B34}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="427167792"/>
+        <c:axId val="331347880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="427167792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="331347880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="331347880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427167792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -22967,6 +23628,46 @@
 </file>
 
 <file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -25907,6 +26608,522 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -31751,6 +32968,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>461817</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>182419</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="차트 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{962B2EE2-273A-425F-875B-04A356870AE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -34582,7 +35837,7 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A19"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -35424,32 +36679,32 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.9140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="28" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="B3" s="28"/>
       <c r="D3" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="25" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="B4" s="25">
         <v>0.62828681920299223</v>
@@ -35460,7 +36715,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="25" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="B5" s="25">
         <v>0.39474432718421348</v>
@@ -35471,7 +36726,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="25" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="B6" s="25">
         <v>0.36952534081688904</v>
@@ -35482,15 +36737,18 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="25" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="B7" s="25">
         <v>0.35062202133007547</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="26" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="B8" s="26">
         <v>51</v>
@@ -35498,30 +36756,30 @@
     </row>
     <row r="10" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="27"/>
       <c r="B11" s="27" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="25" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="B12" s="25">
         <v>2</v>
@@ -35541,7 +36799,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="25" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="B13" s="25">
         <v>48</v>
@@ -35557,7 +36815,7 @@
     </row>
     <row r="14" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="26" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B14" s="26">
         <v>50</v>
@@ -35573,33 +36831,33 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="27"/>
       <c r="B16" s="27" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="H16" s="27" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="25" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B17" s="25">
         <v>-0.70218597546652739</v>
@@ -35695,13 +36953,13 @@
         <v>116</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>117</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
@@ -36390,8 +37648,8 @@
         <v>0.71996216569531635</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A75" s="25">
+    <row r="75" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A75" s="26">
         <v>50</v>
       </c>
       <c r="B75" s="25">
@@ -36405,9 +37663,6 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A76" s="26">
-        <v>51</v>
-      </c>
       <c r="B76" s="26">
         <v>-0.99785682521378105</v>
       </c>
@@ -36430,11 +37685,11 @@
   <dimension ref="A1:AN52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="V58" activePane="bottomRight" state="frozen"/>
       <selection activeCell="I44" sqref="F44:I55"/>
       <selection pane="topRight" activeCell="I44" sqref="F44:I55"/>
       <selection pane="bottomLeft" activeCell="I44" sqref="F44:I55"/>
-      <selection pane="bottomRight" activeCell="AR48" sqref="AR48"/>
+      <selection pane="bottomRight" activeCell="AV71" sqref="AV71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -41949,7 +43204,7 @@
         <f t="shared" si="6"/>
         <v>44014</v>
       </c>
-      <c r="AJ43" s="41">
+      <c r="AJ43" s="32">
         <v>0</v>
       </c>
       <c r="AK43">
@@ -43156,16 +44411,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="40.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="35">
         <v>44014</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -43176,138 +44431,138 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="36"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="32"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="7"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="32"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="7"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="7"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="32"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="7"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="28.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="32"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="7"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="100.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="37" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="7"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" s="36"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="32"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="7"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="32"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="7"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="29.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="36"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="7"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="36"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="32"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="7"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="36"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="32"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="7"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -43323,16 +44578,16 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="34">
         <v>2018</v>
       </c>
       <c r="E15" s="7"/>
@@ -43341,60 +44596,60 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" s="36"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="7"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A17" s="36"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="7"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="36"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="7"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="36"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="7"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A20" s="36"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="7"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -43410,16 +44665,16 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="38" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="33">
         <v>44018</v>
       </c>
       <c r="E22" s="19"/>
@@ -43428,55 +44683,55 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A23" s="37"/>
+      <c r="A23" s="38"/>
       <c r="B23" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="32"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="33"/>
       <c r="E23" s="19"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A24" s="37"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="32"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="19"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A25" s="37"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="32"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="19"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A26" s="37"/>
+      <c r="A26" s="38"/>
       <c r="B26" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="32"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="19"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="38"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="20" t="s">
         <v>87</v>
       </c>

</xml_diff>